<commit_message>
Edited Roster to include more information
</commit_message>
<xml_diff>
--- a/Roster.xlsx
+++ b/Roster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielrevier/Projects/demmies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{409CD836-9509-014B-AF2D-46B42C93F802}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A056A248-9C20-6640-98AE-F11254EF30B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18940" yWindow="8320" windowWidth="28040" windowHeight="17440" xr2:uid="{B8622510-66A6-6140-8878-0BD5A0E2A35E}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{B8622510-66A6-6140-8878-0BD5A0E2A35E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
   <si>
     <t>Delaney</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Drafter</t>
   </si>
   <si>
-    <t>Price Drafted</t>
-  </si>
-  <si>
     <t>Date Dropped</t>
   </si>
   <si>
@@ -130,6 +127,27 @@
   </si>
   <si>
     <t>Kevin K</t>
+  </si>
+  <si>
+    <t>Initial Bid</t>
+  </si>
+  <si>
+    <t>Final Bid</t>
+  </si>
+  <si>
+    <t>Draft Order</t>
+  </si>
+  <si>
+    <t>Bidder</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Messam</t>
+  </si>
+  <si>
+    <t>Swalwell</t>
   </si>
 </sst>
 </file>
@@ -171,10 +189,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,337 +508,571 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F35B05-47E6-9740-B6AF-5FA1D1456242}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="1">
-        <v>42</v>
+        <v>6</v>
+      </c>
+      <c r="B2" s="1">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1">
+        <v>20</v>
+      </c>
+      <c r="F3" s="1">
+        <v>72</v>
+      </c>
+      <c r="G3" s="2">
+        <v>43770</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="1">
+        <v>20</v>
+      </c>
+      <c r="F4" s="1">
+        <v>90</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="1">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="1">
+        <v>60</v>
+      </c>
+      <c r="F5" s="1">
+        <v>60</v>
+      </c>
+      <c r="G5" s="2">
+        <v>43728</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1">
+        <v>50</v>
+      </c>
+      <c r="F6" s="1">
+        <v>95</v>
+      </c>
+      <c r="G6" s="2">
+        <v>43843</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1">
+        <v>2</v>
+      </c>
+      <c r="F7" s="1">
         <v>38</v>
       </c>
-      <c r="D3" s="2">
+      <c r="G7" s="2">
         <v>43801</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1">
+        <v>74</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="1">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="1">
+        <v>15</v>
+      </c>
+      <c r="F9" s="1">
+        <v>30</v>
+      </c>
+      <c r="G9" s="2">
+        <v>43832</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" s="1">
+        <v>42</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="1">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>51</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="1">
+        <v>14</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1">
+        <v>66</v>
+      </c>
+      <c r="G12" s="2">
+        <v>43705</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1">
-        <v>43</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="F13" s="1">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1">
-        <v>66</v>
-      </c>
-      <c r="D5" s="2">
-        <v>43705</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1">
-        <v>135</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="2">
-        <v>43700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="1">
-        <v>72</v>
-      </c>
-      <c r="D9" s="2">
-        <v>43770</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="1">
-        <v>95</v>
-      </c>
-      <c r="D10" s="2">
-        <v>43843</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="1">
-        <v>18</v>
-      </c>
-      <c r="D11" s="2">
-        <v>43762</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="1">
-        <v>3</v>
-      </c>
-      <c r="D12" s="2">
+      <c r="G13" s="2">
         <v>43683</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="1">
-        <v>90</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="1">
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1">
+        <v>16</v>
+      </c>
+      <c r="F14" s="1">
         <v>78</v>
       </c>
-      <c r="D14" s="2">
+      <c r="G14" s="2">
         <v>43802</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="1">
+      <c r="B15" s="1">
+        <v>18</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="1">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1">
         <v>15</v>
       </c>
-      <c r="D15" s="2">
+      <c r="G15" s="2">
         <v>43692</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="1">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="1">
+        <v>2</v>
+      </c>
+      <c r="F16" s="1">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2">
+        <v>43698</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17" s="1">
+        <v>12</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>43</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+      <c r="F18" s="1">
+        <v>1</v>
+      </c>
+      <c r="G18" s="2">
+        <v>43700</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="1">
         <v>17</v>
       </c>
-      <c r="D16" s="2">
-        <v>43840</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="1">
-        <v>59</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="1">
-        <v>30</v>
-      </c>
-      <c r="D18" s="2">
-        <v>43832</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="1">
-        <v>60</v>
-      </c>
-      <c r="D19" s="2">
-        <v>43728</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="1">
+        <v>2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>18</v>
+      </c>
+      <c r="G19" s="2">
+        <v>43762</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C20" s="1">
-        <v>51</v>
+        <v>4</v>
+      </c>
+      <c r="B20" s="1">
+        <v>4</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20" s="1">
+        <v>30</v>
+      </c>
+      <c r="F20" s="1">
+        <v>135</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="B21" s="1">
+        <v>3</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="1">
+        <v>50</v>
+      </c>
+      <c r="F21" s="1">
         <v>111</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="G21" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" s="1">
-        <v>74</v>
+        <v>14</v>
+      </c>
+      <c r="B22" s="1">
+        <v>19</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+      <c r="E22" s="1">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1">
+        <v>17</v>
+      </c>
+      <c r="G22" s="2">
+        <v>43840</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="1">
-        <v>13</v>
-      </c>
-      <c r="D23" s="2">
-        <v>43698</v>
+        <v>15</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="1">
+        <v>10</v>
+      </c>
+      <c r="F23" s="1">
+        <v>59</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="3">
+        <v>43789</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="3">
+        <v>43654</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G23">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update roster dropout dates
</commit_message>
<xml_diff>
--- a/Roster.xlsx
+++ b/Roster.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielrevier/Projects/demmies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFDED37-0C45-304B-A121-84576CEEF48E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97E379-86D8-5041-BBCC-3C494DE1FEBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{B8622510-66A6-6140-8878-0BD5A0E2A35E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>Delaney</t>
   </si>
@@ -511,7 +511,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,8 +558,8 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
+      <c r="G2" s="2">
+        <v>43872</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -696,8 +696,8 @@
       <c r="F8" s="1">
         <v>74</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>26</v>
+      <c r="G8" s="2">
+        <v>43891</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -903,8 +903,8 @@
       <c r="F17" s="1">
         <v>43</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>26</v>
+      <c r="G17" s="2">
+        <v>43892</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1041,8 +1041,8 @@
       <c r="F23" s="1">
         <v>59</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>26</v>
+      <c r="G23" s="2">
+        <v>43872</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update drops in roster
</commit_message>
<xml_diff>
--- a/Roster.xlsx
+++ b/Roster.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielrevier/Projects/demmies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFDED37-0C45-304B-A121-84576CEEF48E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97E379-86D8-5041-BBCC-3C494DE1FEBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{B8622510-66A6-6140-8878-0BD5A0E2A35E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>Delaney</t>
   </si>
@@ -511,7 +511,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -558,8 +558,8 @@
       <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>26</v>
+      <c r="G2" s="2">
+        <v>43872</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -696,8 +696,8 @@
       <c r="F8" s="1">
         <v>74</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>26</v>
+      <c r="G8" s="2">
+        <v>43891</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -903,8 +903,8 @@
       <c r="F17" s="1">
         <v>43</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>26</v>
+      <c r="G17" s="2">
+        <v>43892</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -1041,8 +1041,8 @@
       <c r="F23" s="1">
         <v>59</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>26</v>
+      <c r="G23" s="2">
+        <v>43872</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update for Warren dropping out
</commit_message>
<xml_diff>
--- a/Roster.xlsx
+++ b/Roster.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielrevier/Projects/demmies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD97E379-86D8-5041-BBCC-3C494DE1FEBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3E691B-D393-9949-B09D-8E02445E30A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="17540" xr2:uid="{B8622510-66A6-6140-8878-0BD5A0E2A35E}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="39">
   <si>
     <t>Delaney</t>
   </si>
@@ -511,7 +511,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -995,8 +995,8 @@
       <c r="F21" s="1">
         <v>111</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>26</v>
+      <c r="G21" s="2">
+        <v>43895</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>